<commit_message>
Remove region column (handled by the trans file)
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_IND_CCS.xlsx
+++ b/SubRES_TMPL/SubRes_IND_CCS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EECD022-F623-4ADE-8BE3-9554B6874C2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACDA303-96D2-4E76-9A81-24E19BDAC8C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{ECBB1353-5603-4DB8-AAB9-778C2920C8D3}">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{ECBB1353-5603-4DB8-AAB9-778C2920C8D3}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{DDD152C8-0145-480B-B7AD-E696DA215FB4}">
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{DDD152C8-0145-480B-B7AD-E696DA215FB4}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{C86BAE19-1D7E-4C26-A8E1-349CF00AEC80}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{C86BAE19-1D7E-4C26-A8E1-349CF00AEC80}">
       <text>
         <r>
           <rPr>
@@ -114,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{CCF374F8-3E50-4D7E-9E5E-D717AC9428A5}">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{CCF374F8-3E50-4D7E-9E5E-D717AC9428A5}">
       <text>
         <r>
           <rPr>
@@ -138,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{918B8C5B-665F-49BB-B8C0-6CC6B828346E}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{918B8C5B-665F-49BB-B8C0-6CC6B828346E}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{9193C206-03D9-4D37-948A-9FC18CD486E5}">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{9193C206-03D9-4D37-948A-9FC18CD486E5}">
       <text>
         <r>
           <rPr>
@@ -186,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{47EBD077-2F59-41B5-8B9F-A119259D5A78}">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{47EBD077-2F59-41B5-8B9F-A119259D5A78}">
       <text>
         <r>
           <rPr>
@@ -210,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{10943837-6419-4BC1-BA73-4EA33A83E1B1}">
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{10943837-6419-4BC1-BA73-4EA33A83E1B1}">
       <text>
         <r>
           <rPr>
@@ -234,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{34CA0637-EDFF-4EC8-B432-C4105788F0A7}">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{34CA0637-EDFF-4EC8-B432-C4105788F0A7}">
       <text>
         <r>
           <rPr>
@@ -258,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{8913CADA-9B0D-4630-AEBB-D76E40CC8CBE}">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{8913CADA-9B0D-4630-AEBB-D76E40CC8CBE}">
       <text>
         <r>
           <rPr>
@@ -282,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{5766B56E-8706-4411-B11F-69579DAD7C49}">
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{5766B56E-8706-4411-B11F-69579DAD7C49}">
       <text>
         <r>
           <rPr>
@@ -311,7 +311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Document type:</t>
   </si>
@@ -394,9 +394,6 @@
     <t>Industry</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
     <t>*TechDesc</t>
   </si>
   <si>
@@ -412,9 +409,6 @@
     <t>SHARE-I~UP~0</t>
   </si>
   <si>
-    <t>*Region Name</t>
-  </si>
-  <si>
     <t>Input Commodity</t>
   </si>
   <si>
@@ -439,9 +433,6 @@
     <t>I/E rule</t>
   </si>
   <si>
-    <t>IE,National</t>
-  </si>
-  <si>
     <t>INDCOA</t>
   </si>
   <si>
@@ -518,6 +509,9 @@
   </si>
   <si>
     <t>Cap2Act</t>
+  </si>
+  <si>
+    <t>*Technology Name</t>
   </si>
 </sst>
 </file>
@@ -2319,7 +2313,7 @@
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1">
       <c r="A17" s="34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
@@ -2610,397 +2604,376 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E65932-8AD8-48FB-989E-7D3601E44567}">
-  <dimension ref="A3:V23"/>
+  <dimension ref="A3:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11" style="16" customWidth="1"/>
-    <col min="6" max="12" width="12.28515625" style="16" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="16"/>
-    <col min="15" max="15" width="10.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="67.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="9.42578125" style="16" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="14.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" style="16" customWidth="1"/>
+    <col min="5" max="11" width="12.28515625" style="16" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="16"/>
+    <col min="14" max="14" width="15.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="67.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="9.42578125" style="16" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" style="16" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22">
-      <c r="A3"/>
+    <row r="3" spans="1:20">
+      <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="D3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
-      <c r="L3"/>
-      <c r="N3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="15"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
       <c r="P3" s="20"/>
       <c r="Q3" s="20"/>
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-    </row>
-    <row r="4" spans="1:22" ht="30.75" thickBot="1">
+    </row>
+    <row r="4" spans="1:20" ht="30.75" thickBot="1">
       <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>7</v>
-      </c>
       <c r="F4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>30</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>68</v>
       </c>
       <c r="J4" s="27" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="51">
+      <c r="A5" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="51">
-      <c r="A5" s="28" t="s">
+      <c r="D5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="E5" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="O5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="28" t="s">
+      <c r="P5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="S5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="T5" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="U5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="V5" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
-        <v>40</v>
-      </c>
+      <c r="F6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="J6" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" s="19" t="s">
         <v>57</v>
       </c>
+      <c r="M6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
       <c r="R6" s="19"/>
       <c r="S6" s="19"/>
       <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="16" t="s">
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="16" t="str">
+        <f>N7</f>
+        <v>I-DMD-ONM-N1</v>
+      </c>
+      <c r="B7" s="16" t="str">
+        <f>O7</f>
+        <v>New tech: Other non-metallic mineral products demand process with CCS</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>50</v>
+      </c>
+      <c r="G7" s="16">
+        <v>2030</v>
+      </c>
+      <c r="H7" s="16">
+        <v>1</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0.20479</v>
+      </c>
+      <c r="J7" s="16">
+        <v>5</v>
+      </c>
+      <c r="K7" s="22">
+        <f>510/6.2/$J$23</f>
+        <v>95.560019186952857</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="C8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="16" t="str">
-        <f>P7</f>
-        <v>I-DMD-ONM-N1</v>
-      </c>
-      <c r="C7" s="16" t="str">
-        <f>Q7</f>
-        <v>New tech: Other non-metallic mineral products demand process with CCS</v>
-      </c>
-      <c r="D7" s="16" t="s">
+      <c r="I8" s="21">
+        <v>4.0299999999999997E-3</v>
+      </c>
+      <c r="J8" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="C9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="I9" s="21">
+        <v>5.77E-3</v>
+      </c>
+      <c r="J9" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="C10" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="16">
-        <v>50</v>
-      </c>
-      <c r="H7" s="16">
-        <v>2030</v>
-      </c>
-      <c r="I7" s="16">
-        <v>1</v>
-      </c>
-      <c r="J7" s="21">
-        <v>0.20479</v>
-      </c>
-      <c r="K7" s="16">
+      <c r="I10" s="21">
+        <v>7.0239999999999997E-2</v>
+      </c>
+      <c r="J10" s="16">
         <v>5</v>
       </c>
-      <c r="L7" s="22">
-        <f>510/6.2/$K$23</f>
-        <v>95.560019186952857</v>
-      </c>
-      <c r="N7" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q7" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="R7" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="S7" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="D8" s="16" t="s">
+    </row>
+    <row r="11" spans="1:20">
+      <c r="C11" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="21">
-        <v>4.0299999999999997E-3</v>
-      </c>
-      <c r="K8" s="16">
+      <c r="I11" s="21">
+        <v>0.30934</v>
+      </c>
+      <c r="J11" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
-      <c r="D9" s="16" t="s">
+    <row r="12" spans="1:20">
+      <c r="C12" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="21">
-        <v>5.77E-3</v>
-      </c>
-      <c r="K9" s="16">
+      <c r="I12" s="21">
+        <v>4.8550000000000003E-2</v>
+      </c>
+      <c r="J12" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
-      <c r="D10" s="16" t="s">
+    <row r="13" spans="1:20">
+      <c r="C13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="21">
-        <v>7.0239999999999997E-2</v>
-      </c>
-      <c r="K10" s="16">
+      <c r="I13" s="21">
+        <v>0.12726000000000001</v>
+      </c>
+      <c r="J13" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
-      <c r="D11" s="16" t="s">
+    <row r="14" spans="1:20">
+      <c r="C14" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="21">
-        <v>0.30934</v>
-      </c>
-      <c r="K11" s="16">
+      <c r="I14" s="21">
+        <v>5.2499999999999995E-3</v>
+      </c>
+      <c r="J14" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
-      <c r="D12" s="16" t="s">
+    <row r="15" spans="1:20">
+      <c r="C15" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="21">
-        <v>4.8550000000000003E-2</v>
-      </c>
-      <c r="K12" s="16">
+      <c r="I15" s="21">
+        <v>9.5879999999999993E-2</v>
+      </c>
+      <c r="J15" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
-      <c r="D13" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="21">
-        <v>0.12726000000000001</v>
-      </c>
-      <c r="K13" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="D14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="21">
-        <v>5.2499999999999995E-3</v>
-      </c>
-      <c r="K14" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="D15" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" s="21">
-        <v>9.5879999999999993E-2</v>
-      </c>
-      <c r="K15" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:20">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30" t="s">
-        <v>53</v>
-      </c>
+      <c r="C16" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="31">
+      <c r="I16" s="31">
         <v>0.12894</v>
       </c>
-      <c r="K16" s="30">
+      <c r="J16" s="30">
         <v>5</v>
       </c>
-      <c r="L16" s="30"/>
-    </row>
-    <row r="22" spans="10:12">
-      <c r="J22" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="10:12">
-      <c r="J23" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K23" s="25">
+      <c r="K16" s="30"/>
+    </row>
+    <row r="22" spans="9:11">
+      <c r="I22" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="9:11">
+      <c r="I23" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" s="25">
         <v>0.86080000000000001</v>
       </c>
-      <c r="L23" s="26" t="s">
-        <v>64</v>
+      <c r="K23" s="26" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IND error fix: use NCAP_TLIFE instead of Lifetime (invalid alias); use TIMES attributes instead of their aliases
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_IND_CCS.xlsx
+++ b/SubRES_TMPL/SubRes_IND_CCS.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACDA303-96D2-4E76-9A81-24E19BDAC8C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E116880-A44C-42ED-9FB2-2E965229FE53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
   </bookViews>
@@ -311,7 +311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Document type:</t>
   </si>
@@ -388,9 +388,6 @@
     <t>Operational Commodity Group</t>
   </si>
   <si>
-    <t>INVCOST</t>
-  </si>
-  <si>
     <t>Industry</t>
   </si>
   <si>
@@ -502,16 +499,22 @@
     <t>TIMES-Ireland Industry</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>Start year</t>
   </si>
   <si>
-    <t>Cap2Act</t>
-  </si>
-  <si>
     <t>*Technology Name</t>
+  </si>
+  <si>
+    <t>NCAP_TLIFE</t>
+  </si>
+  <si>
+    <t>NCAP_START</t>
+  </si>
+  <si>
+    <t>PRC_CAPACT</t>
+  </si>
+  <si>
+    <t>NCAP_COST</t>
   </si>
 </sst>
 </file>
@@ -2313,7 +2316,7 @@
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1">
       <c r="A17" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
@@ -2378,7 +2381,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
@@ -2607,7 +2610,7 @@
   <dimension ref="A3:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2615,7 +2618,13 @@
     <col min="1" max="1" width="14.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="16" customWidth="1"/>
-    <col min="5" max="11" width="12.28515625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="17" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="16" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="16" customWidth="1"/>
     <col min="12" max="13" width="9.140625" style="16"/>
     <col min="14" max="14" width="15.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="67.7109375" style="16" bestFit="1" customWidth="1"/>
@@ -2630,7 +2639,7 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -2655,34 +2664,34 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="27" t="s">
+      <c r="J4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="27" t="s">
-        <v>31</v>
-      </c>
       <c r="K4" s="27" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>8</v>
@@ -2711,35 +2720,35 @@
     </row>
     <row r="5" spans="1:20" ht="51">
       <c r="A5" s="28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="E5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="F5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="G5" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H5" s="28"/>
       <c r="I5" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M5" s="17" t="s">
         <v>16</v>
@@ -2768,26 +2777,26 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
@@ -2807,10 +2816,10 @@
         <v>New tech: Other non-metallic mineral products demand process with CCS</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>41</v>
       </c>
       <c r="E7" s="16">
         <v>1</v>
@@ -2835,19 +2844,19 @@
         <v>95.560019186952857</v>
       </c>
       <c r="M7" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O7" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P7" s="32" t="s">
         <v>3</v>
       </c>
       <c r="Q7" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R7" s="32"/>
       <c r="S7" s="32"/>
@@ -2855,7 +2864,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="C8" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="21">
         <v>4.0299999999999997E-3</v>
@@ -2866,7 +2875,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="C9" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="21">
         <v>5.77E-3</v>
@@ -2877,7 +2886,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="C10" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I10" s="21">
         <v>7.0239999999999997E-2</v>
@@ -2888,7 +2897,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="C11" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I11" s="21">
         <v>0.30934</v>
@@ -2899,7 +2908,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="C12" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="21">
         <v>4.8550000000000003E-2</v>
@@ -2910,7 +2919,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="C13" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I13" s="21">
         <v>0.12726000000000001</v>
@@ -2921,7 +2930,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="C14" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I14" s="21">
         <v>5.2499999999999995E-3</v>
@@ -2932,7 +2941,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="C15" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" s="21">
         <v>9.5879999999999993E-2</v>
@@ -2945,7 +2954,7 @@
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
@@ -2962,18 +2971,18 @@
     </row>
     <row r="22" spans="9:11">
       <c r="I22" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="9:11">
       <c r="I23" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J23" s="25">
         <v>0.86080000000000001</v>
       </c>
       <c r="K23" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>